<commit_message>
Dan mail and subject and file name changes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="174">
   <si>
     <t>TableName</t>
   </si>
@@ -38,508 +38,502 @@
     <t>Florida</t>
   </si>
   <si>
-    <t>2024-03-13 10:30:21.777</t>
+    <t>2024-03-17 09:30:25.237</t>
   </si>
   <si>
     <t>San Antonio</t>
   </si>
   <si>
-    <t>2024-03-13 10:30:41.41</t>
-  </si>
-  <si>
-    <t>master.Units_Fact</t>
+    <t>2024-03-17 09:30:51.327</t>
+  </si>
+  <si>
+    <t>dbo.Vendor</t>
+  </si>
+  <si>
+    <t>Kansas City</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:44:26.63</t>
+  </si>
+  <si>
+    <t>Washington DC</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:52:15.52</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:26:19.683</t>
+  </si>
+  <si>
+    <t>California PFW</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:26:23.183</t>
+  </si>
+  <si>
+    <t>Chattanooga</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:26:27.713</t>
+  </si>
+  <si>
+    <t>Boise</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:04.78</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:06.36</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:07.177</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:09.443</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:17.81</t>
+  </si>
+  <si>
+    <t>Little Rock</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:17.977</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:18.56</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:19.283</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:24.003</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:26.383</t>
+  </si>
+  <si>
+    <t>Tulsa</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:30.23</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:14.31</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:25.253</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:07.113</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:09.34</t>
+  </si>
+  <si>
+    <t>Dallas/Fort Worth</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:23.77</t>
+  </si>
+  <si>
+    <t>Lake Havasu</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:36.103</t>
+  </si>
+  <si>
+    <t>OKC</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:43.007</t>
+  </si>
+  <si>
+    <t>Spokane</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:43.38</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:45.413</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:29.49</t>
+  </si>
+  <si>
+    <t>Idaho Falls</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:33.2</t>
+  </si>
+  <si>
+    <t>Institutional Accounts (IAG)</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:35.33</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:37.773</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:39.293</t>
+  </si>
+  <si>
+    <t>Savannah</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:48:42.913</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:44:26.643</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:52:14.56</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:56:13.157</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:53.523</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:20:56.22</t>
   </si>
   <si>
     <t>North Carolina</t>
   </si>
   <si>
-    <t>2024-03-13 07:53:18.857</t>
-  </si>
-  <si>
-    <t>dbo.Vendor</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:34.113</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:07:00.777</t>
-  </si>
-  <si>
-    <t>Kansas City</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:31:33.4</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:31:55.373</t>
-  </si>
-  <si>
-    <t>Little Rock</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:29.637</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:50.48</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:56:50.753</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:46:02.18</t>
-  </si>
-  <si>
-    <t>Savannah</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:46:02.41</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:57:48.17</t>
-  </si>
-  <si>
-    <t>Tulsa</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:57:04.28</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:59:23.35</t>
-  </si>
-  <si>
-    <t>Idaho Falls</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:59:20.29</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:59:27.837</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:58:51.013</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:06:52.913</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:06:55.777</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:06:56.11</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:07:05.73</t>
-  </si>
-  <si>
-    <t>Chattanooga</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:28.563</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:29.313</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:06:38.597</t>
-  </si>
-  <si>
-    <t>Dallas/Fort Worth</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:06:47.887</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:06:48.267</t>
-  </si>
-  <si>
-    <t>OKC</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:07:04.15</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:07:06.38</t>
-  </si>
-  <si>
-    <t>Lake Havasu</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:28:31.393</t>
-  </si>
-  <si>
-    <t>Washington DC</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:31:34.7</t>
-  </si>
-  <si>
-    <t>Boise</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:15:36.973</t>
-  </si>
-  <si>
-    <t>Spokane</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:28:31.58</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:16:00.047</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:16:12.1</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:16:12.24</t>
-  </si>
-  <si>
-    <t>Austin</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:16:13.563</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:28:26.317</t>
-  </si>
-  <si>
-    <t>Institutional Accounts (IAG)</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:46:00.747</t>
-  </si>
-  <si>
-    <t>California PFW</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:52:06.19</t>
+    <t>2024-03-17 06:29:39.707</t>
   </si>
   <si>
     <t>dbo.Underwriting_Fact</t>
   </si>
   <si>
-    <t>2024-03-13 07:44:03.52</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:13.633</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:15.45</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:11.703</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:14.35</t>
+    <t>2024-03-17 07:24:10.557</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:11.49</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:53.86</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:51:08.223</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:11:56.31</t>
+  </si>
+  <si>
+    <t>Colorado Springs</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:12:02.56</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:51:03.707</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:51:12.66</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:25:26.497</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:28:00.223</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:12:01.967</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:12:56.81</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:12:58.403</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:08.077</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:10.823</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:13.123</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:13.733</t>
   </si>
   <si>
     <t>New Jersey</t>
   </si>
   <si>
-    <t>2024-03-13 07:44:10.3</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:11.487</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:12.49</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:18.687</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:50:56.92</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:03:09.447</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:12:12.14</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:13:19.793</t>
+    <t>2024-03-17 07:13:14.123</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:20.577</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:27.493</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:28.457</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:31.013</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:13:31.453</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:07.43</t>
   </si>
   <si>
     <t>Columbia - St Louis</t>
   </si>
   <si>
-    <t>2024-03-13 07:02:53.29</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:11:49.733</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:11:43.46</t>
+    <t>2024-03-17 07:45:07.563</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:07.927</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:09.037</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:45:09.14</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:40:43.483</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:40:48.273</t>
   </si>
   <si>
     <t>Maine</t>
   </si>
   <si>
-    <t>2024-03-13 06:29:40.257</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:12:07.99</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:29:39.74</t>
-  </si>
-  <si>
-    <t>2024-03-13 08:14:31.913</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:31.23</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:41.283</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:02.723</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:54:31.257</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:54:34.527</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:54:35.57</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:03.087</t>
-  </si>
-  <si>
-    <t>Colorado Springs</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:03.937</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:05.76</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:44:06.84</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:01.263</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:02.083</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:03.2</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:04.103</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:54:19.07</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:53:51.777</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:55:01.72</t>
+    <t>2024-03-17 07:40:49.54</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:54.363</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:55.083</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:55.57</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:55.94</t>
+  </si>
+  <si>
+    <t>2024-03-17 07:24:58.337</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:20:06.193</t>
   </si>
   <si>
     <t>dbo.LeaseRenewals</t>
   </si>
   <si>
-    <t>2024-03-13 06:53:14.41</t>
+    <t>2024-03-17 06:43:59.543</t>
   </si>
   <si>
     <t>dbo.BuildingManagementFees</t>
   </si>
   <si>
-    <t>2024-03-13 06:25:43.25</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:25:44.137</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:26:58.36</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:27:16.033</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:27:31.24</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:47:30.357</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:49:06.313</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:39.77</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:19:28.12</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:50:09.887</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:51:10.14</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:45:41.973</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:47:21.22</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:47:53.51</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:48:41.4</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:50:09.8</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:19:43.593</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:18:33.41</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:18:43.17</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:19:04.207</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:41.833</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:15.223</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:23:28.897</t>
+    <t>2024-03-17 06:02:04.7</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:07:55.133</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:08:04.19</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:08:34.49</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:08:53.703</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:09:07.993</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:14:05.313</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:09:45.077</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:10:26.217</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:13:10.72</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:01:57.503</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:04:47.05</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:05:38.333</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:05:38.66</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:05:54.557</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:05:58.223</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:13:06.773</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:03:35.103</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:03:42.947</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:14:23.03</t>
   </si>
   <si>
     <t>Chicago PFW</t>
   </si>
   <si>
-    <t>2024-03-13 06:25:43.743</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:25:49.023</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:26:55.243</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:45:13.88</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:45:56.3</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:47:10.153</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:49:52.53</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:47:27.84</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:48:13.133</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:48:26.753</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:48:36.487</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:49:01.193</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:49:04.263</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:51:15.46</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:15:16.317</t>
-  </si>
-  <si>
-    <t>2024-03-13 07:41:16.6</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:19:15.637</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:21:22.183</t>
-  </si>
-  <si>
-    <t>2024-03-13 06:21:25.667</t>
+    <t>2024-03-17 06:05:40.2</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:06:00.31</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:13:03.66</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:14:25.867</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:09:23.907</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:09:31.69</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:09:41.35</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:11:47.23</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:11:48.19</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:11:53.99</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:12:13.69</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:12:27.483</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:12:30.347</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:12:48.063</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:12:56.297</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:04:03.337</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:04:10.937</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:04:25.7</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:09:37.56</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:11:37.143</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:11:39.25</t>
+  </si>
+  <si>
+    <t>2024-03-17 06:12:21.23</t>
   </si>
   <si>
     <t>dbo.AuditLogDeletions</t>
   </si>
   <si>
-    <t>2024-03-13 06:12:44.683</t>
+    <t>2024-03-17 06:00:16.393</t>
   </si>
 </sst>
 </file>
@@ -584,7 +578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -621,10 +615,10 @@
         <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>697.0</v>
+        <v>806.0</v>
       </c>
       <c r="E2" t="n">
-        <v>697.0</v>
+        <v>806.0</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -641,10 +635,10 @@
         <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>430.0</v>
+        <v>440.0</v>
       </c>
       <c r="E3" t="n">
-        <v>430.0</v>
+        <v>440.0</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -658,13 +652,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>5698.0</v>
+        <v>613.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5697.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>5697.0</v>
+        <v>0.0</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -672,39 +666,39 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="n">
+        <v>535.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1737.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>1990.0</v>
+        <v>841.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -712,19 +706,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>612.0</v>
+        <v>928.0</v>
       </c>
       <c r="D7" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -732,19 +726,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" t="n">
-        <v>821.0</v>
+        <v>140.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
@@ -752,13 +746,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="n">
-        <v>78.0</v>
+        <v>1191.0</v>
       </c>
       <c r="D9" t="n">
         <v>1.0</v>
@@ -772,19 +766,19 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
       </c>
       <c r="C10" t="n">
-        <v>991.0</v>
+        <v>992.0</v>
       </c>
       <c r="D10" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="F10" t="s">
         <v>25</v>
@@ -792,19 +786,19 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="n">
-        <v>1173.0</v>
+        <v>209.0</v>
       </c>
       <c r="D11" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="E11" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
@@ -812,19 +806,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
       <c r="C12" t="n">
-        <v>803.0</v>
+        <v>499.0</v>
       </c>
       <c r="D12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F12" t="s">
         <v>29</v>
@@ -832,13 +826,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
       <c r="C13" t="n">
-        <v>37.0</v>
+        <v>1753.0</v>
       </c>
       <c r="D13" t="n">
         <v>1.0</v>
@@ -852,19 +846,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>209.0</v>
+        <v>78.0</v>
       </c>
       <c r="D14" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E14" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F14" t="s">
         <v>33</v>
@@ -872,19 +866,19 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="n">
-        <v>715.0</v>
+        <v>249.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E15" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F15" t="s">
         <v>35</v>
@@ -892,19 +886,19 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>36</v>
       </c>
       <c r="C16" t="n">
-        <v>1498.0</v>
+        <v>311.0</v>
       </c>
       <c r="D16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F16" t="s">
         <v>37</v>
@@ -912,19 +906,19 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
       </c>
       <c r="C17" t="n">
-        <v>804.0</v>
+        <v>1498.0</v>
       </c>
       <c r="D17" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
@@ -932,19 +926,19 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>1140.0</v>
+        <v>464.0</v>
       </c>
       <c r="D18" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="E18" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="F18" t="s">
         <v>41</v>
@@ -952,19 +946,19 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
       </c>
       <c r="C19" t="n">
-        <v>311.0</v>
+        <v>716.0</v>
       </c>
       <c r="D19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F19" t="s">
         <v>43</v>
@@ -972,19 +966,19 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20" t="n">
-        <v>2337.0</v>
+        <v>2340.0</v>
       </c>
       <c r="D20" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E20" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F20" t="s">
         <v>45</v>
@@ -992,19 +986,19 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
       </c>
       <c r="C21" t="n">
-        <v>1753.0</v>
+        <v>579.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E21" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F21" t="s">
         <v>47</v>
@@ -1012,19 +1006,19 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
       <c r="C22" t="n">
-        <v>249.0</v>
+        <v>100.0</v>
       </c>
       <c r="D22" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="E22" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="F22" t="s">
         <v>49</v>
@@ -1032,173 +1026,173 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C23" t="n">
-        <v>877.0</v>
+        <v>1173.0</v>
       </c>
       <c r="D23" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E23" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" t="n">
-        <v>140.0</v>
+        <v>4908.0</v>
       </c>
       <c r="D24" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E24" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" t="n">
-        <v>358.0</v>
+        <v>244.0</v>
       </c>
       <c r="D25" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E25" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" t="n">
-        <v>100.0</v>
+        <v>1113.0</v>
       </c>
       <c r="D26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" t="n">
-        <v>4908.0</v>
+        <v>263.0</v>
       </c>
       <c r="D27" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E27" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" t="n">
-        <v>499.0</v>
+        <v>1141.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E28" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" t="n">
-        <v>1113.0</v>
+        <v>2033.0</v>
       </c>
       <c r="D29" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E29" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="F29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30" t="n">
-        <v>464.0</v>
+        <v>805.0</v>
       </c>
       <c r="D30" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E30" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31" t="n">
-        <v>242.0</v>
+        <v>1604.0</v>
       </c>
       <c r="D31" t="n">
         <v>2.0</v>
@@ -1207,84 +1201,84 @@
         <v>2.0</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C32" t="n">
-        <v>535.0</v>
+        <v>703.0</v>
       </c>
       <c r="D32" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E32" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C33" t="n">
-        <v>1191.0</v>
+        <v>803.0</v>
       </c>
       <c r="D33" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="E33" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="F33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" t="n">
-        <v>263.0</v>
+        <v>37.0</v>
       </c>
       <c r="D34" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E34" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="C35" t="n">
-        <v>578.0</v>
+        <v>6951.0</v>
       </c>
       <c r="D35" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E35" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F35" t="s">
         <v>74</v>
@@ -1292,19 +1286,19 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C36" t="n">
-        <v>6949.0</v>
+        <v>879.0</v>
       </c>
       <c r="D36" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="E36" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="F36" t="s">
         <v>75</v>
@@ -1312,19 +1306,19 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
         <v>76</v>
       </c>
       <c r="C37" t="n">
-        <v>703.0</v>
+        <v>358.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E37" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F37" t="s">
         <v>77</v>
@@ -1332,19 +1326,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
         <v>78</v>
       </c>
       <c r="C38" t="n">
-        <v>841.0</v>
+        <v>821.0</v>
       </c>
       <c r="D38" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="E38" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F38" t="s">
         <v>79</v>
@@ -1352,19 +1346,19 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
         <v>80</v>
       </c>
       <c r="C39" t="n">
-        <v>2031.0</v>
+        <v>1737.0</v>
       </c>
       <c r="D39" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="E39" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F39" t="s">
         <v>81</v>
@@ -1372,19 +1366,19 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
         <v>82</v>
       </c>
       <c r="C40" t="n">
-        <v>1604.0</v>
+        <v>1990.0</v>
       </c>
       <c r="D40" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E40" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F40" t="s">
         <v>83</v>
@@ -1392,19 +1386,19 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="C41" t="n">
-        <v>928.0</v>
+        <v>114.0</v>
       </c>
       <c r="D41" t="n">
-        <v>7.0</v>
+        <v>114.0</v>
       </c>
       <c r="E41" t="n">
-        <v>7.0</v>
+        <v>593.0</v>
       </c>
       <c r="F41" t="s">
         <v>85</v>
@@ -1412,99 +1406,99 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>220.0</v>
+      </c>
+      <c r="F42" t="s">
         <v>86</v>
-      </c>
-      <c r="B42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="D42" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="E42" t="n">
-        <v>154.0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C43" t="n">
-        <v>104.0</v>
+        <v>50.0</v>
       </c>
       <c r="D43" t="n">
-        <v>104.0</v>
+        <v>50.0</v>
       </c>
       <c r="E43" t="n">
-        <v>470.0</v>
+        <v>491.0</v>
       </c>
       <c r="F43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C44" t="n">
-        <v>87.0</v>
+        <v>12.0</v>
       </c>
       <c r="D44" t="n">
-        <v>87.0</v>
+        <v>12.0</v>
       </c>
       <c r="E44" t="n">
-        <v>333.0</v>
+        <v>92.0</v>
       </c>
       <c r="F44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C45" t="n">
-        <v>24.0</v>
+        <v>57.0</v>
       </c>
       <c r="D45" t="n">
-        <v>24.0</v>
+        <v>57.0</v>
       </c>
       <c r="E45" t="n">
-        <v>56.0</v>
+        <v>232.0</v>
       </c>
       <c r="F45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="C46" t="n">
-        <v>202.0</v>
+        <v>15.0</v>
       </c>
       <c r="D46" t="n">
-        <v>202.0</v>
+        <v>15.0</v>
       </c>
       <c r="E46" t="n">
-        <v>579.0</v>
+        <v>95.0</v>
       </c>
       <c r="F46" t="s">
         <v>91</v>
@@ -1512,30 +1506,30 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>167.0</v>
+      </c>
+      <c r="F47" t="s">
         <v>92</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E47" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="F47" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C48" t="n">
         <v>109.0</v>
@@ -1544,578 +1538,578 @@
         <v>109.0</v>
       </c>
       <c r="E48" t="n">
-        <v>348.0</v>
+        <v>591.0</v>
       </c>
       <c r="F48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C49" t="n">
-        <v>114.0</v>
+        <v>294.0</v>
       </c>
       <c r="D49" t="n">
-        <v>114.0</v>
+        <v>294.0</v>
       </c>
       <c r="E49" t="n">
-        <v>578.0</v>
+        <v>1527.0</v>
       </c>
       <c r="F49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C50" t="n">
-        <v>12.0</v>
+        <v>95.0</v>
       </c>
       <c r="D50" t="n">
-        <v>12.0</v>
+        <v>95.0</v>
       </c>
       <c r="E50" t="n">
-        <v>65.0</v>
+        <v>280.0</v>
       </c>
       <c r="F50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>3.0</v>
+        <v>187.0</v>
       </c>
       <c r="D51" t="n">
-        <v>3.0</v>
+        <v>187.0</v>
       </c>
       <c r="E51" t="n">
-        <v>4.0</v>
+        <v>573.0</v>
       </c>
       <c r="F51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="C52" t="n">
-        <v>192.0</v>
+        <v>314.0</v>
       </c>
       <c r="D52" t="n">
-        <v>192.0</v>
+        <v>314.0</v>
       </c>
       <c r="E52" t="n">
-        <v>865.0</v>
+        <v>1028.0</v>
       </c>
       <c r="F52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="C53" t="n">
-        <v>29.0</v>
+        <v>22.0</v>
       </c>
       <c r="D53" t="n">
-        <v>29.0</v>
+        <v>22.0</v>
       </c>
       <c r="E53" t="n">
-        <v>158.0</v>
+        <v>53.0</v>
       </c>
       <c r="F53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C54" t="n">
-        <v>235.0</v>
+        <v>85.0</v>
       </c>
       <c r="D54" t="n">
-        <v>235.0</v>
+        <v>85.0</v>
       </c>
       <c r="E54" t="n">
-        <v>740.0</v>
+        <v>329.0</v>
       </c>
       <c r="F54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C55" t="n">
-        <v>22.0</v>
+        <v>72.0</v>
       </c>
       <c r="D55" t="n">
-        <v>22.0</v>
+        <v>72.0</v>
       </c>
       <c r="E55" t="n">
-        <v>232.0</v>
+        <v>355.0</v>
       </c>
       <c r="F55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C56" t="n">
-        <v>16.0</v>
+        <v>124.0</v>
       </c>
       <c r="D56" t="n">
-        <v>16.0</v>
+        <v>124.0</v>
       </c>
       <c r="E56" t="n">
-        <v>65.0</v>
+        <v>727.0</v>
       </c>
       <c r="F56" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C57" t="n">
-        <v>279.0</v>
+        <v>9.0</v>
       </c>
       <c r="D57" t="n">
-        <v>279.0</v>
+        <v>9.0</v>
       </c>
       <c r="E57" t="n">
-        <v>1481.0</v>
+        <v>10.0</v>
       </c>
       <c r="F57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" t="n">
-        <v>14.0</v>
+        <v>1.0</v>
       </c>
       <c r="D58" t="n">
-        <v>14.0</v>
+        <v>1.0</v>
       </c>
       <c r="E58" t="n">
-        <v>113.0</v>
+        <v>30.0</v>
       </c>
       <c r="F58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C59" t="n">
-        <v>17.0</v>
+        <v>123.0</v>
       </c>
       <c r="D59" t="n">
-        <v>17.0</v>
+        <v>123.0</v>
       </c>
       <c r="E59" t="n">
-        <v>102.0</v>
+        <v>501.0</v>
       </c>
       <c r="F59" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C60" t="n">
-        <v>16.0</v>
+        <v>135.0</v>
       </c>
       <c r="D60" t="n">
-        <v>16.0</v>
+        <v>135.0</v>
       </c>
       <c r="E60" t="n">
-        <v>172.0</v>
+        <v>376.0</v>
       </c>
       <c r="F60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C61" t="n">
-        <v>3.0</v>
+        <v>40.0</v>
       </c>
       <c r="D61" t="n">
-        <v>3.0</v>
+        <v>40.0</v>
       </c>
       <c r="E61" t="n">
-        <v>15.0</v>
+        <v>181.0</v>
       </c>
       <c r="F61" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="C62" t="n">
-        <v>48.0</v>
+        <v>108.0</v>
       </c>
       <c r="D62" t="n">
-        <v>48.0</v>
+        <v>108.0</v>
       </c>
       <c r="E62" t="n">
-        <v>508.0</v>
+        <v>494.0</v>
       </c>
       <c r="F62" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C63" t="n">
-        <v>112.0</v>
+        <v>10.0</v>
       </c>
       <c r="D63" t="n">
-        <v>112.0</v>
+        <v>10.0</v>
       </c>
       <c r="E63" t="n">
-        <v>476.0</v>
+        <v>62.0</v>
       </c>
       <c r="F63" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C64" t="n">
-        <v>66.0</v>
+        <v>21.0</v>
       </c>
       <c r="D64" t="n">
-        <v>66.0</v>
+        <v>21.0</v>
       </c>
       <c r="E64" t="n">
-        <v>358.0</v>
+        <v>149.0</v>
       </c>
       <c r="F64" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="C65" t="n">
-        <v>35.0</v>
+        <v>22.0</v>
       </c>
       <c r="D65" t="n">
-        <v>35.0</v>
+        <v>22.0</v>
       </c>
       <c r="E65" t="n">
-        <v>157.0</v>
+        <v>231.0</v>
       </c>
       <c r="F65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C66" t="n">
-        <v>293.0</v>
+        <v>25.0</v>
       </c>
       <c r="D66" t="n">
-        <v>293.0</v>
+        <v>25.0</v>
       </c>
       <c r="E66" t="n">
-        <v>1001.0</v>
+        <v>88.0</v>
       </c>
       <c r="F66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C67" t="n">
-        <v>77.0</v>
+        <v>110.0</v>
       </c>
       <c r="D67" t="n">
-        <v>77.0</v>
+        <v>110.0</v>
       </c>
       <c r="E67" t="n">
-        <v>309.0</v>
+        <v>261.0</v>
       </c>
       <c r="F67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C68" t="n">
-        <v>42.0</v>
+        <v>21.0</v>
       </c>
       <c r="D68" t="n">
-        <v>42.0</v>
+        <v>21.0</v>
       </c>
       <c r="E68" t="n">
-        <v>220.0</v>
+        <v>174.0</v>
       </c>
       <c r="F68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>22</v>
       </c>
       <c r="C69" t="n">
-        <v>20.0</v>
+        <v>285.0</v>
       </c>
       <c r="D69" t="n">
-        <v>20.0</v>
+        <v>285.0</v>
       </c>
       <c r="E69" t="n">
-        <v>100.0</v>
+        <v>787.0</v>
       </c>
       <c r="F69" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C70" t="n">
-        <v>111.0</v>
+        <v>194.0</v>
       </c>
       <c r="D70" t="n">
-        <v>111.0</v>
+        <v>194.0</v>
       </c>
       <c r="E70" t="n">
-        <v>259.0</v>
+        <v>886.0</v>
       </c>
       <c r="F70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="C71" t="n">
-        <v>120.0</v>
+        <v>9.0</v>
       </c>
       <c r="D71" t="n">
-        <v>120.0</v>
+        <v>9.0</v>
       </c>
       <c r="E71" t="n">
-        <v>716.0</v>
+        <v>98.0</v>
       </c>
       <c r="F71" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C72" t="n">
-        <v>62.0</v>
+        <v>28.0</v>
       </c>
       <c r="D72" t="n">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="E72" t="n">
-        <v>331.0</v>
+        <v>79.0</v>
       </c>
       <c r="F72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C73" t="n">
-        <v>23.0</v>
+        <v>86.0</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0</v>
+        <v>86.0</v>
       </c>
       <c r="E73" t="n">
-        <v>78.0</v>
+        <v>385.0</v>
       </c>
       <c r="F73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C74" t="n">
-        <v>49.0</v>
+        <v>37.0</v>
       </c>
       <c r="D74" t="n">
-        <v>49.0</v>
+        <v>37.0</v>
       </c>
       <c r="E74" t="n">
-        <v>147.0</v>
+        <v>137.0</v>
       </c>
       <c r="F74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C75" t="n">
-        <v>85.0</v>
+        <v>3.0</v>
       </c>
       <c r="D75" t="n">
-        <v>85.0</v>
+        <v>3.0</v>
       </c>
       <c r="E75" t="n">
-        <v>265.0</v>
+        <v>16.0</v>
       </c>
       <c r="F75" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C76" t="n">
-        <v>105.0</v>
+        <v>115.0</v>
       </c>
       <c r="D76" t="n">
-        <v>105.0</v>
+        <v>115.0</v>
       </c>
       <c r="E76" t="n">
-        <v>568.0</v>
+        <v>365.0</v>
       </c>
       <c r="F76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C77" t="n">
         <v>21.0</v>
@@ -2124,27 +2118,27 @@
         <v>21.0</v>
       </c>
       <c r="E77" t="n">
-        <v>84.0</v>
+        <v>74.0</v>
       </c>
       <c r="F77" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B78" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C78" t="n">
-        <v>34.0</v>
+        <v>21000.0</v>
       </c>
       <c r="D78" t="n">
-        <v>34.0</v>
+        <v>21000.0</v>
       </c>
       <c r="E78" t="n">
-        <v>207.0</v>
+        <v>20993.0</v>
       </c>
       <c r="F78" t="s">
         <v>127</v>
@@ -2155,16 +2149,16 @@
         <v>128</v>
       </c>
       <c r="B79" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C79" t="n">
-        <v>20983.0</v>
+        <v>21625.0</v>
       </c>
       <c r="D79" t="n">
-        <v>20983.0</v>
+        <v>7359.0</v>
       </c>
       <c r="E79" t="n">
-        <v>20976.0</v>
+        <v>3220.0</v>
       </c>
       <c r="F79" t="s">
         <v>129</v>
@@ -2172,399 +2166,399 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" t="n">
+        <v>135046.0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>21947.0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>8324.0</v>
+      </c>
+      <c r="F80" t="s">
         <v>130</v>
-      </c>
-      <c r="B80" t="s">
-        <v>80</v>
-      </c>
-      <c r="C80" t="n">
-        <v>135043.0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>32968.0</v>
-      </c>
-      <c r="E80" t="n">
-        <v>9865.0</v>
-      </c>
-      <c r="F80" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C81" t="n">
-        <v>17182.0</v>
+        <v>33065.0</v>
       </c>
       <c r="D81" t="n">
-        <v>2647.0</v>
+        <v>6301.0</v>
       </c>
       <c r="E81" t="n">
-        <v>720.0</v>
+        <v>91.0</v>
       </c>
       <c r="F81" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C82" t="n">
-        <v>88338.0</v>
+        <v>10855.0</v>
       </c>
       <c r="D82" t="n">
-        <v>14882.0</v>
+        <v>798.0</v>
       </c>
       <c r="E82" t="n">
-        <v>6098.0</v>
+        <v>204.0</v>
       </c>
       <c r="F82" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B83" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C83" t="n">
-        <v>23289.0</v>
+        <v>219940.0</v>
       </c>
       <c r="D83" t="n">
-        <v>5862.0</v>
+        <v>38162.0</v>
       </c>
       <c r="E83" t="n">
-        <v>3212.0</v>
+        <v>6191.0</v>
       </c>
       <c r="F83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B84" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C84" t="n">
-        <v>128688.0</v>
+        <v>39694.0</v>
       </c>
       <c r="D84" t="n">
-        <v>22095.0</v>
+        <v>5179.0</v>
       </c>
       <c r="E84" t="n">
-        <v>9319.0</v>
+        <v>2332.0</v>
       </c>
       <c r="F84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B85" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C85" t="n">
-        <v>3799.0</v>
+        <v>70000.0</v>
       </c>
       <c r="D85" t="n">
-        <v>691.0</v>
+        <v>15886.0</v>
       </c>
       <c r="E85" t="n">
-        <v>270.0</v>
+        <v>2937.0</v>
       </c>
       <c r="F85" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C86" t="n">
-        <v>34479.0</v>
+        <v>4926.0</v>
       </c>
       <c r="D86" t="n">
-        <v>10058.0</v>
+        <v>1045.0</v>
       </c>
       <c r="E86" t="n">
-        <v>4837.0</v>
+        <v>36.0</v>
       </c>
       <c r="F86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C87" t="n">
-        <v>370.0</v>
+        <v>95428.0</v>
       </c>
       <c r="D87" t="n">
-        <v>67.0</v>
+        <v>15742.0</v>
       </c>
       <c r="E87" t="n">
-        <v>32.0</v>
+        <v>3286.0</v>
       </c>
       <c r="F87" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B88" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C88" t="n">
-        <v>18360.0</v>
+        <v>9467.0</v>
       </c>
       <c r="D88" t="n">
-        <v>1014.0</v>
+        <v>2478.0</v>
       </c>
       <c r="E88" t="n">
-        <v>650.0</v>
+        <v>89.0</v>
       </c>
       <c r="F88" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B89" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C89" t="n">
-        <v>394.0</v>
+        <v>77407.0</v>
       </c>
       <c r="D89" t="n">
-        <v>0.0</v>
+        <v>3729.0</v>
       </c>
       <c r="E89" t="n">
-        <v>0.0</v>
+        <v>644.0</v>
       </c>
       <c r="F89" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C90" t="n">
-        <v>24753.0</v>
+        <v>25790.0</v>
       </c>
       <c r="D90" t="n">
-        <v>6604.0</v>
+        <v>52.0</v>
       </c>
       <c r="E90" t="n">
-        <v>3398.0</v>
+        <v>0.0</v>
       </c>
       <c r="F90" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B91" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C91" t="n">
-        <v>27192.0</v>
+        <v>7534.0</v>
       </c>
       <c r="D91" t="n">
-        <v>3603.0</v>
+        <v>3053.0</v>
       </c>
       <c r="E91" t="n">
-        <v>693.0</v>
+        <v>0.0</v>
       </c>
       <c r="F91" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B92" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C92" t="n">
-        <v>25970.0</v>
+        <v>61183.0</v>
       </c>
       <c r="D92" t="n">
-        <v>6945.0</v>
+        <v>8861.0</v>
       </c>
       <c r="E92" t="n">
-        <v>1806.0</v>
+        <v>2750.0</v>
       </c>
       <c r="F92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B93" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C93" t="n">
-        <v>31051.0</v>
+        <v>370.0</v>
       </c>
       <c r="D93" t="n">
-        <v>22734.0</v>
+        <v>62.0</v>
       </c>
       <c r="E93" t="n">
-        <v>11418.0</v>
+        <v>0.0</v>
       </c>
       <c r="F93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B94" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="C94" t="n">
-        <v>15157.0</v>
+        <v>18420.0</v>
       </c>
       <c r="D94" t="n">
-        <v>2429.0</v>
+        <v>3880.0</v>
       </c>
       <c r="E94" t="n">
-        <v>1350.0</v>
+        <v>245.0</v>
       </c>
       <c r="F94" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B95" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C95" t="n">
-        <v>4913.0</v>
+        <v>24819.0</v>
       </c>
       <c r="D95" t="n">
-        <v>813.0</v>
+        <v>5658.0</v>
       </c>
       <c r="E95" t="n">
-        <v>217.0</v>
+        <v>1598.0</v>
       </c>
       <c r="F95" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C96" t="n">
-        <v>61183.0</v>
+        <v>58952.0</v>
       </c>
       <c r="D96" t="n">
-        <v>18553.0</v>
+        <v>26768.0</v>
       </c>
       <c r="E96" t="n">
-        <v>2688.0</v>
+        <v>138.0</v>
       </c>
       <c r="F96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B97" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="C97" t="n">
-        <v>7534.0</v>
+        <v>17224.0</v>
       </c>
       <c r="D97" t="n">
-        <v>1569.0</v>
+        <v>2507.0</v>
       </c>
       <c r="E97" t="n">
-        <v>428.0</v>
+        <v>20.0</v>
       </c>
       <c r="F97" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B98" t="s">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="C98" t="n">
-        <v>12307.0</v>
+        <v>2342.0</v>
       </c>
       <c r="D98" t="n">
-        <v>3262.0</v>
+        <v>520.0</v>
       </c>
       <c r="E98" t="n">
-        <v>1261.0</v>
+        <v>29.0</v>
       </c>
       <c r="F98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B99" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="C99" t="n">
-        <v>77387.0</v>
+        <v>3830.0</v>
       </c>
       <c r="D99" t="n">
-        <v>5863.0</v>
+        <v>3830.0</v>
       </c>
       <c r="E99" t="n">
-        <v>1278.0</v>
+        <v>0.0</v>
       </c>
       <c r="F99" t="s">
         <v>150</v>
@@ -2572,19 +2566,19 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B100" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="C100" t="n">
-        <v>18420.0</v>
+        <v>128727.0</v>
       </c>
       <c r="D100" t="n">
-        <v>6706.0</v>
+        <v>22178.0</v>
       </c>
       <c r="E100" t="n">
-        <v>1258.0</v>
+        <v>5121.0</v>
       </c>
       <c r="F100" t="s">
         <v>151</v>
@@ -2592,19 +2586,19 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C101" t="n">
-        <v>58952.0</v>
+        <v>15157.0</v>
       </c>
       <c r="D101" t="n">
-        <v>25088.0</v>
+        <v>2447.0</v>
       </c>
       <c r="E101" t="n">
-        <v>8106.0</v>
+        <v>900.0</v>
       </c>
       <c r="F101" t="s">
         <v>152</v>
@@ -2612,19 +2606,19 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C102" t="n">
-        <v>25721.0</v>
+        <v>34479.0</v>
       </c>
       <c r="D102" t="n">
-        <v>2555.0</v>
+        <v>10681.0</v>
       </c>
       <c r="E102" t="n">
-        <v>1267.0</v>
+        <v>822.0</v>
       </c>
       <c r="F102" t="s">
         <v>153</v>
@@ -2632,402 +2626,382 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B103" t="s">
+        <v>66</v>
+      </c>
+      <c r="C103" t="n">
+        <v>97219.0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>506.0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F103" t="s">
         <v>154</v>
-      </c>
-      <c r="C103" t="n">
-        <v>3830.0</v>
-      </c>
-      <c r="D103" t="n">
-        <v>3830.0</v>
-      </c>
-      <c r="E103" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F103" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B104" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C104" t="n">
-        <v>33065.0</v>
+        <v>25970.0</v>
       </c>
       <c r="D104" t="n">
-        <v>2727.0</v>
+        <v>4998.0</v>
       </c>
       <c r="E104" t="n">
-        <v>1055.0</v>
+        <v>435.0</v>
       </c>
       <c r="F104" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="C105" t="n">
-        <v>8258.0</v>
+        <v>4199.0</v>
       </c>
       <c r="D105" t="n">
-        <v>1801.0</v>
+        <v>457.0</v>
       </c>
       <c r="E105" t="n">
-        <v>260.0</v>
+        <v>115.0</v>
       </c>
       <c r="F105" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B106" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C106" t="n">
-        <v>25790.0</v>
+        <v>11403.0</v>
       </c>
       <c r="D106" t="n">
-        <v>25.0</v>
+        <v>1636.0</v>
       </c>
       <c r="E106" t="n">
-        <v>25.0</v>
+        <v>43.0</v>
       </c>
       <c r="F106" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B107" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="C107" t="n">
-        <v>21625.0</v>
+        <v>3799.0</v>
       </c>
       <c r="D107" t="n">
-        <v>8758.0</v>
+        <v>733.0</v>
       </c>
       <c r="E107" t="n">
-        <v>3888.0</v>
+        <v>0.0</v>
       </c>
       <c r="F107" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B108" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C108" t="n">
-        <v>95367.0</v>
+        <v>132518.0</v>
       </c>
       <c r="D108" t="n">
-        <v>16444.0</v>
+        <v>18199.0</v>
       </c>
       <c r="E108" t="n">
-        <v>4495.0</v>
+        <v>3018.0</v>
       </c>
       <c r="F108" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B109" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C109" t="n">
-        <v>4199.0</v>
+        <v>31183.0</v>
       </c>
       <c r="D109" t="n">
-        <v>435.0</v>
+        <v>15573.0</v>
       </c>
       <c r="E109" t="n">
-        <v>69.0</v>
+        <v>3861.0</v>
       </c>
       <c r="F109" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B110" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C110" t="n">
-        <v>11403.0</v>
+        <v>394.0</v>
       </c>
       <c r="D110" t="n">
-        <v>2011.0</v>
+        <v>0.0</v>
       </c>
       <c r="E110" t="n">
-        <v>980.0</v>
+        <v>0.0</v>
       </c>
       <c r="F110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B111" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C111" t="n">
-        <v>10832.0</v>
+        <v>23307.0</v>
       </c>
       <c r="D111" t="n">
-        <v>858.0</v>
+        <v>5372.0</v>
       </c>
       <c r="E111" t="n">
-        <v>324.0</v>
+        <v>1621.0</v>
       </c>
       <c r="F111" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B112" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="C112" t="n">
-        <v>219831.0</v>
+        <v>24625.0</v>
       </c>
       <c r="D112" t="n">
-        <v>40162.0</v>
+        <v>6287.0</v>
       </c>
       <c r="E112" t="n">
-        <v>12420.0</v>
+        <v>240.0</v>
       </c>
       <c r="F112" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B113" t="s">
         <v>9</v>
       </c>
       <c r="C113" t="n">
-        <v>54501.0</v>
+        <v>54535.0</v>
       </c>
       <c r="D113" t="n">
-        <v>13128.0</v>
+        <v>13432.0</v>
       </c>
       <c r="E113" t="n">
-        <v>5711.0</v>
+        <v>3813.0</v>
       </c>
       <c r="F113" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B114" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C114" t="n">
-        <v>58553.0</v>
+        <v>25721.0</v>
       </c>
       <c r="D114" t="n">
-        <v>7398.0</v>
+        <v>2241.0</v>
       </c>
       <c r="E114" t="n">
-        <v>2815.0</v>
+        <v>179.0</v>
       </c>
       <c r="F114" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B115" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C115" t="n">
-        <v>2342.0</v>
+        <v>12307.0</v>
       </c>
       <c r="D115" t="n">
-        <v>375.0</v>
+        <v>2662.0</v>
       </c>
       <c r="E115" t="n">
-        <v>166.0</v>
+        <v>140.0</v>
       </c>
       <c r="F115" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B116" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C116" t="n">
-        <v>9450.0</v>
+        <v>27192.0</v>
       </c>
       <c r="D116" t="n">
-        <v>2077.0</v>
+        <v>1630.0</v>
       </c>
       <c r="E116" t="n">
-        <v>673.0</v>
+        <v>609.0</v>
       </c>
       <c r="F116" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B117" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="C117" t="n">
-        <v>69967.0</v>
+        <v>8258.0</v>
       </c>
       <c r="D117" t="n">
-        <v>21144.0</v>
+        <v>1101.0</v>
       </c>
       <c r="E117" t="n">
-        <v>6781.0</v>
+        <v>0.0</v>
       </c>
       <c r="F117" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B118" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="C118" t="n">
-        <v>97219.0</v>
+        <v>88466.0</v>
       </c>
       <c r="D118" t="n">
-        <v>44.0</v>
+        <v>18797.0</v>
       </c>
       <c r="E118" t="n">
-        <v>22.0</v>
+        <v>2291.0</v>
       </c>
       <c r="F118" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B119" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C119" t="n">
-        <v>39694.0</v>
+        <v>18360.0</v>
       </c>
       <c r="D119" t="n">
-        <v>5587.0</v>
+        <v>1482.0</v>
       </c>
       <c r="E119" t="n">
-        <v>2950.0</v>
+        <v>728.0</v>
       </c>
       <c r="F119" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B120" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C120" t="n">
-        <v>132491.0</v>
+        <v>58633.0</v>
       </c>
       <c r="D120" t="n">
-        <v>21393.0</v>
+        <v>8980.0</v>
       </c>
       <c r="E120" t="n">
-        <v>4466.0</v>
+        <v>1922.0</v>
       </c>
       <c r="F120" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="B121" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C121" t="n">
-        <v>24625.0</v>
+        <v>13955.0</v>
       </c>
       <c r="D121" t="n">
-        <v>6463.0</v>
+        <v>30.0</v>
       </c>
       <c r="E121" t="n">
-        <v>2795.0</v>
+        <v>30.0</v>
       </c>
       <c r="F121" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="s">
-        <v>174</v>
-      </c>
-      <c r="B122" t="s">
-        <v>12</v>
-      </c>
-      <c r="C122" t="n">
-        <v>13868.0</v>
-      </c>
-      <c r="D122" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="E122" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="F122" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>